<commit_message>
adicionando matriz de rigidez e tentativa de jacobi e gauss-seidel
</commit_message>
<xml_diff>
--- a/trelica.xlsx
+++ b/trelica.xlsx
@@ -300,7 +300,7 @@
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.66"/>
   </cols>
@@ -409,10 +409,10 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="11.66"/>
   </cols>
@@ -456,7 +456,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>3</v>
@@ -473,10 +473,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="n">
         <v>3</v>
-      </c>
-      <c r="B4" s="4" t="n">
-        <v>1</v>
       </c>
       <c r="C4" s="9" t="n">
         <v>210000000000</v>
@@ -543,7 +543,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>6</v>
@@ -557,7 +557,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>6</v>
@@ -571,10 +571,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7" t="n">
         <v>7</v>
-      </c>
-      <c r="B11" s="7" t="n">
-        <v>4</v>
       </c>
       <c r="C11" s="9" t="n">
         <v>210000000000</v>
@@ -585,10 +585,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7" t="n">
         <v>7</v>
-      </c>
-      <c r="B12" s="7" t="n">
-        <v>6</v>
       </c>
       <c r="C12" s="9" t="n">
         <v>210000000000</v>
@@ -599,10 +599,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B13" s="7" t="n">
         <v>8</v>
-      </c>
-      <c r="B13" s="7" t="n">
-        <v>7</v>
       </c>
       <c r="C13" s="9" t="n">
         <v>210000000000</v>
@@ -613,10 +613,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B14" s="7" t="n">
         <v>8</v>
-      </c>
-      <c r="B14" s="7" t="n">
-        <v>6</v>
       </c>
       <c r="C14" s="9" t="n">
         <v>210000000000</v>
@@ -655,7 +655,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="11.66"/>
   </cols>
@@ -872,7 +872,7 @@
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.66"/>
   </cols>

</xml_diff>